<commit_message>
very good model. 1_2
</commit_message>
<xml_diff>
--- a/controllers/CL_TEST_8_action 5/data/Curriculum Yes new model_1_2/Curriculum Yes new model_1_2_Test_heterogeineous_pipe_1/Curriculum Yes new model_1_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
+++ b/controllers/CL_TEST_8_action 5/data/Curriculum Yes new model_1_2/Curriculum Yes new model_1_2_Test_heterogeineous_pipe_1/Curriculum Yes new model_1_2_Test_heterogeineous_pipe_1_Test_Result.xlsx
@@ -445,16 +445,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>395</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>0.9875</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0075</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>